<commit_message>
Updated date format in daily performance, removed org type and retrieve from leave type, implemented staffid non mandatory and changed error message
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Bulk Shift Extension Import.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Bulk Shift Extension Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\internship041\source\repos\VLead Attendance Management System\Vlead\AttendanceManagement\wwwroot\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B18824-B831-489B-A348-F58058B14BE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0272F-3B35-42D7-AF22-271F35B842BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -548,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7247F6-9FB1-4AF9-B5F2-F91777127E52}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>